<commit_message>
Working on silkscreen and ordering
</commit_message>
<xml_diff>
--- a/Mixer Board/TS3A5017-Mixer/Manufacture/TS3A5017-Mixer-BOM.xlsx
+++ b/Mixer Board/TS3A5017-Mixer/Manufacture/TS3A5017-Mixer-BOM.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brokebit/Sync/KiCad/SDR-Learning-Project/Mixer Board/TS3A5017-Mixer/Manufacture/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4ABE10FD-6652-FF47-BB1E-B70BD65D6FF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86334011-A246-4240-9862-B232FE0D52B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="69000" yWindow="9180" windowWidth="27640" windowHeight="16940" xr2:uid="{D9076A68-DDB4-F644-AAB4-15BDA0A7F9C6}"/>
+    <workbookView xWindow="2300" yWindow="10460" windowWidth="34560" windowHeight="20620" xr2:uid="{D9076A68-DDB4-F644-AAB4-15BDA0A7F9C6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="TS3A5017_Mixer" localSheetId="0">Sheet1!$A$1:$E$8</definedName>
+    <definedName name="TS3A5017_Mixer" localSheetId="0">Sheet1!$A$1:$E$5</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -41,7 +41,7 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
   <connection id="1" xr16:uid="{D336C909-160B-1044-83C5-A1E6E99F17AB}" name="TS3A5017-Mixer" type="6" refreshedVersion="8" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/brokebit/Sync/KiCad/SDR-Learning-Project/Mixer Board/TS3A5017-Mixer/Manufacture/TS3A5017-Mixer.csv" tab="0" semicolon="1">
+    <textPr sourceFile="/Users/brokebit/Sync/KiCad/SDR-Learning-Project/Mixer Board/TS3A5017-Mixer/Manufacture/TS3A5017-Mixer.csv" tab="0" semicolon="1">
       <textFields count="8">
         <textField/>
         <textField/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
   <si>
     <t>Designator</t>
   </si>
@@ -66,61 +66,94 @@
     <t>Footprint</t>
   </si>
   <si>
+    <t>U1</t>
+  </si>
+  <si>
+    <t>Texas_RGY_R-PVQFN-N16_EP2.05x2.55mm</t>
+  </si>
+  <si>
+    <t>TS3A5017RGY</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>C_0603_1608Metric</t>
+  </si>
+  <si>
+    <t>.1uf</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>C4,C5,C10,C9,C3,C12,C6,C8,C13,C11,C2,C7</t>
+  </si>
+  <si>
+    <t>C14,C15</t>
+  </si>
+  <si>
+    <t>R1,R2</t>
+  </si>
+  <si>
+    <t>U2,U3</t>
+  </si>
+  <si>
+    <t>J5</t>
+  </si>
+  <si>
+    <t>C_0201_0603Metric</t>
+  </si>
+  <si>
+    <t>R_0201_0603Metric</t>
+  </si>
+  <si>
+    <t>SOT-23-5</t>
+  </si>
+  <si>
+    <t>HRO_PJ-320D-A</t>
+  </si>
+  <si>
+    <t>1uf</t>
+  </si>
+  <si>
+    <t>10k</t>
+  </si>
+  <si>
+    <t>LMP7715MF</t>
+  </si>
+  <si>
+    <t>PJ-320D-A</t>
+  </si>
+  <si>
+    <t>J3</t>
+  </si>
+  <si>
+    <t>J4</t>
+  </si>
+  <si>
     <t>J1</t>
   </si>
   <si>
-    <t>AMPHENOL_901-143-6RFX</t>
+    <t>J2</t>
+  </si>
+  <si>
+    <t>CLK1</t>
+  </si>
+  <si>
+    <t>Conn_01x02_Pin</t>
   </si>
   <si>
     <t>RF-In</t>
   </si>
   <si>
-    <t>J2</t>
-  </si>
-  <si>
     <t>CLK0</t>
   </si>
   <si>
-    <t>J3</t>
-  </si>
-  <si>
-    <t>CLK1</t>
-  </si>
-  <si>
-    <t>J4</t>
-  </si>
-  <si>
-    <t>PinHeader_1x06_P2.54mm_Vertical</t>
-  </si>
-  <si>
-    <t>Conn_01x06</t>
-  </si>
-  <si>
-    <t>U1</t>
-  </si>
-  <si>
-    <t>Texas_RGY_R-PVQFN-N16_EP2.05x2.55mm</t>
-  </si>
-  <si>
-    <t>TS3A5017RGY</t>
-  </si>
-  <si>
-    <t>C1</t>
-  </si>
-  <si>
-    <t>C_0603_1608Metric</t>
-  </si>
-  <si>
-    <t>.1uf</t>
-  </si>
-  <si>
-    <t>C5,C4,C3,C2</t>
-  </si>
-  <si>
-    <t>C_1206_3216Metric</t>
-  </si>
-  <si>
-    <t>Comment</t>
+    <t>SMA_Amphenol_901-143_Horizontal</t>
+  </si>
+  <si>
+    <t>PinHeader_1x02_P2.54mm_Vertical</t>
   </si>
 </sst>
 </file>
@@ -496,10 +529,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15C5CBFD-9D46-6A43-A98C-EEE2A15B8972}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -511,7 +544,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -522,32 +555,32 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C4" t="s">
         <v>3</v>
@@ -555,46 +588,90 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="C6" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" t="s">
         <v>17</v>
-      </c>
-      <c r="B8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>